<commit_message>
adding FPGA resource utilization
</commit_message>
<xml_diff>
--- a/FPGA/resources.xlsx
+++ b/FPGA/resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>DNN</t>
   </si>
@@ -202,6 +202,132 @@
   </si>
   <si>
     <t>FF</t>
+  </si>
+  <si>
+    <t>Multipliers</t>
+  </si>
+  <si>
+    <t>DFFs</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>width bits</t>
+  </si>
+  <si>
+    <t>Add/Comp</t>
+  </si>
+  <si>
+    <t>1 bit</t>
+  </si>
+  <si>
+    <t>Mult Set</t>
+  </si>
+  <si>
+    <t>Other Modules</t>
+  </si>
+  <si>
+    <t>Adder</t>
+  </si>
+  <si>
+    <t>costterm set</t>
+  </si>
+  <si>
+    <t>z Adders</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Assume max is 4b</t>
+  </si>
+  <si>
+    <t>cycleblockcnt</t>
+  </si>
+  <si>
+    <t>log(cpc-2)</t>
+  </si>
+  <si>
+    <t>MUXes</t>
+  </si>
+  <si>
+    <t>N to 1</t>
+  </si>
+  <si>
+    <t>mux</t>
+  </si>
+  <si>
+    <t>muxset</t>
+  </si>
+  <si>
+    <t>M muxes</t>
+  </si>
+  <si>
+    <t>2N maxfinders</t>
+  </si>
+  <si>
+    <t>DFF</t>
+  </si>
+  <si>
+    <t>width*depth</t>
+  </si>
+  <si>
+    <t>sigmoid table</t>
+  </si>
+  <si>
+    <t>Mem cells</t>
+  </si>
+  <si>
+    <t>Total mem bits</t>
+  </si>
+  <si>
+    <t>Mem each cell</t>
+  </si>
+  <si>
+    <t>sp table</t>
+  </si>
+  <si>
+    <t>interleaverset</t>
+  </si>
+  <si>
+    <t>FF proc</t>
+  </si>
+  <si>
+    <t>z Multipliers</t>
+  </si>
+  <si>
+    <t>z/fi sig functions</t>
+  </si>
+  <si>
+    <t>sig function</t>
+  </si>
+  <si>
+    <t>2*fi+1 Adders (width_TA bits)</t>
+  </si>
+  <si>
+    <t>1 sigmoid table</t>
+  </si>
+  <si>
+    <t>1 sp table</t>
+  </si>
+  <si>
+    <t>BP proc</t>
+  </si>
+  <si>
+    <t>"z" Adders</t>
+  </si>
+  <si>
+    <t>"z" Mulitpliers</t>
+  </si>
+  <si>
+    <t>2z Multipliers</t>
+  </si>
+  <si>
+    <t>UP proc</t>
   </si>
 </sst>
 </file>
@@ -278,12 +404,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -563,13 +691,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -750,6 +884,13 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8">
+        <f>LOG(C7,2)</f>
+        <v>2</v>
+      </c>
       <c r="O8" t="s">
         <v>25</v>
       </c>
@@ -806,7 +947,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>55</v>
       </c>
@@ -818,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -828,6 +969,278 @@
       <c r="D18">
         <f>H2</f>
         <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>1+I2+1+1+I2+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f>1+1+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27">
+        <f>4*2</f>
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f>F27/2</f>
+        <v>4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28">
+        <f>C8*2</f>
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29">
+        <f>H2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>1024</v>
+      </c>
+      <c r="J36">
+        <f>J2</f>
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <f>I36*J36</f>
+        <v>7168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1024</v>
+      </c>
+      <c r="J37">
+        <f>J2-2</f>
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <f>I37*J37</f>
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39">
+        <f>C3*C6*LOG(B2/C6,2)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converting to define notation
and unifying testbenches
</commit_message>
<xml_diff>
--- a/FPGA/resources.xlsx
+++ b/FPGA/resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
   <si>
     <t>DNN</t>
   </si>
@@ -201,9 +201,6 @@
     <t>layers</t>
   </si>
   <si>
-    <t>FF</t>
-  </si>
-  <si>
     <t>Multipliers</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>MUXes</t>
   </si>
   <si>
-    <t>N to 1</t>
-  </si>
-  <si>
     <t>mux</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>Total mem bits</t>
   </si>
   <si>
-    <t>Mem each cell</t>
-  </si>
-  <si>
     <t>sp table</t>
   </si>
   <si>
@@ -328,13 +319,151 @@
   </si>
   <si>
     <t>UP proc</t>
+  </si>
+  <si>
+    <t>Bits each cell</t>
+  </si>
+  <si>
+    <t>32 bit param</t>
+  </si>
+  <si>
+    <t>z + z/fi Multipliers</t>
+  </si>
+  <si>
+    <t>z + z/fi Adders</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>parallel_mem</t>
+  </si>
+  <si>
+    <t>z memory</t>
+  </si>
+  <si>
+    <t>mem_coll</t>
+  </si>
+  <si>
+    <t>collection parallel_mem</t>
+  </si>
+  <si>
+    <t>dual_port_memory</t>
+  </si>
+  <si>
+    <t>Same as above 3</t>
+  </si>
+  <si>
+    <t>w_mem_ctr</t>
+  </si>
+  <si>
+    <t>output SM</t>
+  </si>
+  <si>
+    <t>1 counter</t>
+  </si>
+  <si>
+    <t>hidden SM</t>
+  </si>
+  <si>
+    <t>1 interleaver set</t>
+  </si>
+  <si>
+    <t>1 address_decoder</t>
+  </si>
+  <si>
+    <t>1 act_sp_ctr</t>
+  </si>
+  <si>
+    <t>act_sp_ctr</t>
+  </si>
+  <si>
+    <t>LOTS</t>
+  </si>
+  <si>
+    <t>4 counters</t>
+  </si>
+  <si>
+    <t>10*depth</t>
+  </si>
+  <si>
+    <t>AM coll</t>
+  </si>
+  <si>
+    <t>input SM</t>
+  </si>
+  <si>
+    <t>1 act_ctr</t>
+  </si>
+  <si>
+    <t>act_ctr</t>
+  </si>
+  <si>
+    <t>3 counters</t>
+  </si>
+  <si>
+    <t>address_decoder</t>
+  </si>
+  <si>
+    <t>input layer block</t>
+  </si>
+  <si>
+    <t>dual_port_mem_coll</t>
+  </si>
+  <si>
+    <t>z*coll = 160 memories, each is p/z * width_in = 2*8b</t>
+  </si>
+  <si>
+    <t>z+z/fi = 36 memories, each is p*fo/z * width = 4*10b</t>
+  </si>
+  <si>
+    <t>1 FF_proc</t>
+  </si>
+  <si>
+    <t>1 UP_proc</t>
+  </si>
+  <si>
+    <t>(N*width), N is Nto1</t>
+  </si>
+  <si>
+    <t>hidden layer block</t>
+  </si>
+  <si>
+    <t>2*z*coll = 80 memories, each is p/z * width = 2*10b</t>
+  </si>
+  <si>
+    <t>z+z/fi = 9 mems, each is p*fo/z * width = 4*10b. Also z*coll = 16 mems, each is p/z*width = 2*10b</t>
+  </si>
+  <si>
+    <t>1 BP_proc</t>
+  </si>
+  <si>
+    <t>output layer block</t>
+  </si>
+  <si>
+    <t>1 costterm_set</t>
+  </si>
+  <si>
+    <t>z/fi*coll = 2 memories, each is p/(z/fi) * width = 16*10b</t>
+  </si>
+  <si>
+    <t>1 cycleblockcnt</t>
+  </si>
+  <si>
+    <t>Layers</t>
+  </si>
+  <si>
+    <t>par_dual_port_mem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -371,8 +500,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +525,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -398,13 +539,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -412,10 +606,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -691,18 +894,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -885,7 +1089,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <f>LOG(C7,2)</f>
@@ -900,6 +1104,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
       <c r="N9" t="s">
         <v>27</v>
       </c>
@@ -909,6 +1119,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
       <c r="N10" t="s">
         <v>28</v>
       </c>
@@ -916,334 +1132,710 @@
         <v>130</v>
       </c>
     </row>
+    <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>52</v>
+      <c r="F14">
+        <f>1+I2+1+1+I2+1</f>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
+      <c r="A15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>54</v>
+      <c r="A16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>1+1+1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17">
-        <f>H2*L2</f>
-        <v>30</v>
+      <c r="A17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18">
+      <c r="A18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18">
+        <f>4*2</f>
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <f>F18/2</f>
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19">
+        <f>C8*2</f>
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20">
         <f>H2</f>
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>1024</v>
+      </c>
+      <c r="K27">
+        <f>J2</f>
+        <v>7</v>
+      </c>
+      <c r="L27">
+        <f>J27*K27</f>
+        <v>7168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="J21" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1024</v>
+      </c>
+      <c r="K28">
+        <f>J2-2</f>
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <f>J28*K28</f>
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <f>C3*C6*LOG(B2/C6,2)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K21" t="s">
-        <v>84</v>
-      </c>
-      <c r="N21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <f>1+I2+1+1+I2+1</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <f>1+1+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="6" t="s">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27">
-        <f>4*2</f>
-        <v>8</v>
-      </c>
-      <c r="G27">
-        <f>F27/2</f>
-        <v>4</v>
-      </c>
-      <c r="N27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28">
-        <f>C8*2</f>
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <f>C8</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29">
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>102</v>
+      </c>
+      <c r="K41">
         <f>H2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="L41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H49">
+        <f>E6*C8</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="H50">
+        <f>1 + 2*C8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52">
+        <f>2*C8 + 2*C6*LOG(B2/C6,2)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+      <c r="H53">
+        <f>2*C9 + 2*C6*LOG(C6,2)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="10"/>
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="10"/>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" t="s">
+        <v>124</v>
+      </c>
+      <c r="H56">
+        <f>2*C8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="H57">
+        <f>2*C9+C6*LOG(C6,2)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="10"/>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="11"/>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="F61">
+        <v>8</v>
+      </c>
+      <c r="I61">
+        <f>K2*C6*C9*2+K2*C6*2</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="10"/>
+      <c r="B62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="10"/>
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+      <c r="L63">
+        <f>K2*C9*B2/C6*C6</f>
+        <v>2560</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="10"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="10"/>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="L65">
+        <f>H2*B2*C3/C6*(C6+C6/C5)</f>
+        <v>1440</v>
+      </c>
+      <c r="M65" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="10"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="10"/>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="10"/>
+      <c r="B68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="10"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="I70">
+        <f>3*H2*E6*C9 + 5*H2*E6*E6 + 2*H2*E6*2 + H2*E6</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A71" s="10"/>
+      <c r="B71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A72" s="10"/>
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+      <c r="L72">
+        <f>2*C9*H2*D2/E6*E6</f>
+        <v>1600</v>
+      </c>
+      <c r="M72" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A73" s="10"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="7"/>
+    </row>
+    <row r="74" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="10"/>
+      <c r="B74" t="s">
+        <v>127</v>
+      </c>
+      <c r="L74">
+        <f>H2*D2*E3/E6*(E6+E6/E5) + 2*H2*D2/E6*E6</f>
+        <v>680</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N74" s="7"/>
+      <c r="O74" s="7"/>
+      <c r="P74" s="7"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A75" s="10"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="10"/>
+      <c r="B76" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A77" s="10"/>
+      <c r="B77" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78" s="10"/>
+      <c r="B78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" s="10"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" t="s">
+        <v>110</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <f>CEILING(LOG(C8+2,2),1)+E6/E5*(C7+2)*2</f>
+        <v>14</v>
+      </c>
+      <c r="I80">
+        <f>2*H2*E6/E5</f>
+        <v>20</v>
+      </c>
+      <c r="L80">
+        <f>2*H2*D2/(E6/E5)*E6/E5</f>
+        <v>320</v>
+      </c>
+      <c r="M80" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N80" s="7"/>
+      <c r="O80" s="7"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" s="11"/>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>50</v>
+      </c>
+      <c r="H83">
+        <f>H2*C10+H2</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="10"/>
+      <c r="B84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="10"/>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" s="10"/>
+      <c r="B86" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" s="10"/>
+      <c r="B87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" s="11"/>
+      <c r="B88" t="s">
         <v>54</v>
       </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="G34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="I36">
-        <v>1024</v>
-      </c>
-      <c r="J36">
-        <f>J2</f>
-        <v>7</v>
-      </c>
-      <c r="K36">
-        <f>I36*J36</f>
-        <v>7168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="I37" s="5">
-        <v>1024</v>
-      </c>
-      <c r="J37">
-        <f>J2-2</f>
-        <v>5</v>
-      </c>
-      <c r="K37">
-        <f>I37*J37</f>
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>87</v>
-      </c>
-      <c r="G39">
-        <f>C3*C6*LOG(B2/C6,2)</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>99</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="M80:O81"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="M63:O64"/>
+    <mergeCell ref="M65:O66"/>
+    <mergeCell ref="M72:O73"/>
+    <mergeCell ref="M74:P75"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1252,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="185" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
eta bit shift works now!
also fixing rounding issue in multiplier
</commit_message>
<xml_diff>
--- a/FPGA/resources.xlsx
+++ b/FPGA/resources.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Layer 3</t>
   </si>
   <si>
-    <t>cpc-2</t>
-  </si>
-  <si>
     <t>Should be =</t>
   </si>
   <si>
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>par_dual_port_mem</t>
+  </si>
+  <si>
+    <t>Clocks per cycle - 2</t>
   </si>
 </sst>
 </file>
@@ -606,14 +606,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,25 +926,25 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -977,10 +977,10 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
         <v>17</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
       </c>
       <c r="P2">
         <f>K2*C6/C3</f>
@@ -998,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3">
         <f>E6/E5</f>
@@ -1018,7 +1018,7 @@
         <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P4">
         <f>H2</f>
@@ -1038,7 +1038,7 @@
         <v>8</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -1055,7 +1055,7 @@
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -1063,24 +1063,24 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
       <c r="C7">
         <f>C4/C6</f>
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <f>E4/E6</f>
         <v>4</v>
       </c>
       <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
         <v>23</v>
-      </c>
-      <c r="O7" t="s">
-        <v>24</v>
       </c>
       <c r="P7">
         <f>E6/E5</f>
@@ -1089,14 +1089,14 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <f>LOG(C7,2)</f>
         <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P8">
         <f>F2</f>
@@ -1105,13 +1105,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P9">
         <f>SUM(P2:P8)</f>
@@ -1120,77 +1120,77 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P10" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" t="s">
-        <v>58</v>
-      </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" t="s">
         <v>81</v>
       </c>
-      <c r="K12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" t="s">
-        <v>82</v>
-      </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>59</v>
+      <c r="A14" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1204,16 +1204,16 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>63</v>
+      <c r="A15" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>65</v>
+      <c r="A16" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1224,16 +1224,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>66</v>
+      <c r="A17" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>68</v>
+      <c r="A18" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="F18">
         <f>4*2</f>
@@ -1244,12 +1244,12 @@
         <v>4</v>
       </c>
       <c r="N18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="F19">
         <f>C8*2</f>
@@ -1264,8 +1264,8 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>74</v>
+      <c r="A20" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="I20">
         <f>H2</f>
@@ -1273,27 +1273,27 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>54</v>
+      <c r="A22" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>53</v>
+      <c r="A23" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1303,24 +1303,24 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
         <v>78</v>
       </c>
-      <c r="H24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" t="s">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1338,8 +1338,8 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>83</v>
+      <c r="A28" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1357,8 +1357,8 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>84</v>
+      <c r="A30" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="G30">
         <v>5</v>
@@ -1369,126 +1369,126 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
         <v>88</v>
-      </c>
-      <c r="B32" t="s">
-        <v>89</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="9"/>
+      <c r="B34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="9"/>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="B37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="9"/>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="B39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="B40" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K41">
         <f>H2</f>
         <v>10</v>
       </c>
       <c r="L41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>101</v>
+      <c r="A42" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
         <v>103</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="B44" t="s">
         <v>105</v>
       </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="C45" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="7" t="s">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="H49">
         <f>E6*C8</f>
@@ -1496,11 +1496,11 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
         <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>111</v>
       </c>
       <c r="H50">
         <f>1 + 2*C8</f>
@@ -1508,19 +1508,19 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>125</v>
+      <c r="A51" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" t="s">
         <v>116</v>
-      </c>
-      <c r="B52" t="s">
-        <v>118</v>
-      </c>
-      <c r="E52" t="s">
-        <v>117</v>
       </c>
       <c r="H52">
         <f>2*C8 + 2*C6*LOG(B2/C6,2)</f>
@@ -1528,11 +1528,11 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" t="s">
-        <v>113</v>
       </c>
       <c r="H53">
         <f>2*C9 + 2*C6*LOG(C6,2)</f>
@@ -1540,23 +1540,23 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
+      <c r="A54" s="9"/>
       <c r="B54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+      <c r="B55" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="10"/>
-      <c r="B55" t="s">
-        <v>115</v>
-      </c>
-    </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" t="s">
         <v>123</v>
-      </c>
-      <c r="B56" t="s">
-        <v>124</v>
       </c>
       <c r="H56">
         <f>2*C8</f>
@@ -1564,11 +1564,11 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>121</v>
+      <c r="A57" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H57">
         <f>2*C9+C6*LOG(C6,2)</f>
@@ -1576,23 +1576,23 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
+      <c r="A58" s="9"/>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
+      <c r="A59" s="10"/>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
-        <v>126</v>
+      <c r="A61" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F61">
         <v>8</v>
@@ -1603,74 +1603,74 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="10"/>
+      <c r="A62" s="9"/>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="10"/>
+      <c r="A63" s="9"/>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L63">
         <f>K2*C9*B2/C6*C6</f>
         <v>2560</v>
       </c>
-      <c r="M63" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="N63" s="7"/>
-      <c r="O63" s="7"/>
+      <c r="M63" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="10"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
+      <c r="A64" s="9"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="10"/>
+      <c r="A65" s="9"/>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L65">
         <f>H2*B2*C3/C6*(C6+C6/C5)</f>
         <v>1440</v>
       </c>
-      <c r="M65" s="7" t="s">
+      <c r="M65" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="9"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="9"/>
+      <c r="B67" t="s">
         <v>129</v>
       </c>
-      <c r="N65" s="7"/>
-      <c r="O65" s="7"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="10"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="7"/>
-      <c r="O66" s="7"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="10"/>
-      <c r="B67" t="s">
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="9"/>
+      <c r="B68" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="10"/>
-      <c r="B68" t="s">
-        <v>131</v>
-      </c>
-    </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="10"/>
+      <c r="A69" s="9"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>133</v>
+      <c r="A70" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I70">
         <f>3*H2*E6*C9 + 5*H2*E6*E6 + 2*H2*E6*2 + H2*E6</f>
@@ -1678,82 +1678,82 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="10"/>
+      <c r="A71" s="9"/>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="10"/>
+      <c r="A72" s="9"/>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L72">
         <f>2*C9*H2*D2/E6*E6</f>
         <v>1600</v>
       </c>
-      <c r="M72" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
+      <c r="M72" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" s="10"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
+      <c r="A73" s="9"/>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12"/>
     </row>
     <row r="74" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="10"/>
+      <c r="A74" s="9"/>
       <c r="B74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L74">
         <f>H2*D2*E3/E6*(E6+E6/E5) + 2*H2*D2/E6*E6</f>
         <v>680</v>
       </c>
-      <c r="M74" s="7" t="s">
+      <c r="M74" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12"/>
+      <c r="P74" s="12"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A75" s="9"/>
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12"/>
+      <c r="P75" s="12"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="9"/>
+      <c r="B76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A77" s="9"/>
+      <c r="B77" t="s">
         <v>135</v>
       </c>
-      <c r="N74" s="7"/>
-      <c r="O74" s="7"/>
-      <c r="P74" s="7"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A75" s="10"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A76" s="10"/>
-      <c r="B76" t="s">
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78" s="9"/>
+      <c r="B78" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A77" s="10"/>
-      <c r="B77" t="s">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" s="9"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="10"/>
-      <c r="B78" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="10"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -1770,27 +1770,27 @@
         <f>2*H2*D2/(E6/E5)*E6/E5</f>
         <v>320</v>
       </c>
-      <c r="M80" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="N80" s="7"/>
-      <c r="O80" s="7"/>
+      <c r="M80" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
+      <c r="A81" s="10"/>
       <c r="B81" t="s">
-        <v>138</v>
-      </c>
-      <c r="M81" s="7"/>
-      <c r="N81" s="7"/>
-      <c r="O81" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H83">
         <f>H2*C10+H2</f>
@@ -1798,33 +1798,33 @@
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A84" s="10"/>
+      <c r="A84" s="9"/>
       <c r="B84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="9"/>
+      <c r="B85" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A85" s="10"/>
-      <c r="B85" t="s">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" s="9"/>
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" s="9"/>
+      <c r="B87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A86" s="10"/>
-      <c r="B86" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A87" s="10"/>
-      <c r="B87" t="s">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" s="10"/>
+      <c r="B88" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A88" s="11"/>
-      <c r="B88" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+    <sheetView zoomScale="185" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1856,7 +1856,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>15850</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <f>2^F4</f>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <f>D3*B1</f>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <f>F5*B1</f>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3">
         <v>19000</v>
@@ -1929,19 +1929,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <f>B8*F5/1024</f>
         <v>1187.5</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <f>D2*B1</f>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3">
         <v>135</v>
@@ -1958,10 +1958,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
       </c>
       <c r="D12">
         <v>36</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <f>B11*D12</f>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>210</v>
@@ -1986,18 +1986,18 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="3">
         <v>240</v>

</xml_diff>